<commit_message>
cập nhật thứ tự sprint 2
</commit_message>
<xml_diff>
--- a/File Tài liệu/File kế hoạch gantt/gantt_tổng_có_giao_diện_lẫn_back_end.xlsx
+++ b/File Tài liệu/File kế hoạch gantt/gantt_tổng_có_giao_diện_lẫn_back_end.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Blazor\LmsMini\File Tài liệu\File kế hoạch gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BC23EC-76D8-4416-A6A5-FE387D37DB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830F874A-23DD-41EE-9E5C-293B2715DA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2102,8 +2102,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="168" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -2226,9 +2227,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -2266,17 +2264,20 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="138">
+  <dxfs count="129">
     <dxf>
       <fill>
         <patternFill>
@@ -2554,73 +2555,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBFBFBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2660,6 +2594,32 @@
           <bgColor rgb="FFBFBFBF"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2676,42 +2636,35 @@
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
-        <charset val="163"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2733,6 +2686,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2752,6 +2731,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2771,6 +2776,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2790,30 +2821,166 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="163"/>
+        <scheme val="major"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2847,14 +3014,14 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2880,244 +3047,36 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="163"/>
-        <scheme val="major"/>
-      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="163"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="163"/>
-        <scheme val="major"/>
-      </font>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="163"/>
-        <scheme val="major"/>
-      </font>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="163"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="163"/>
-        <scheme val="major"/>
-      </font>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="163"/>
-        <scheme val="major"/>
-      </font>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="163"/>
-        <scheme val="major"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3134,35 +3093,10 @@
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
+        <charset val="163"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3581,7 +3515,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCBEF2D7-706F-4E36-9A8E-78F9A3847E57}" type="CELLRANGE">
+                    <a:fld id="{5FF38A7F-3586-401E-90ED-DBE106F94638}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3615,7 +3549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{681820A6-1B74-4AAA-AF95-99D6FCBE18BC}" type="CELLRANGE">
+                    <a:fld id="{0E3A0237-1DBF-48D7-9E02-1292410E0AB1}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3649,7 +3583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E76AD74F-CDE8-4188-B41E-D8579CB8BD89}" type="CELLRANGE">
+                    <a:fld id="{7BB055E6-3272-4683-97E0-21440E7E940C}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3683,7 +3617,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E8C8C09-B440-4490-BE86-722A3905261B}" type="CELLRANGE">
+                    <a:fld id="{F4471BFE-2A98-4B28-8E03-7027255F727F}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3717,7 +3651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE4058D4-04F7-488F-A6AA-E3EC793BC842}" type="CELLRANGE">
+                    <a:fld id="{6B965ADF-1DFC-4347-AAAA-5310FDCB1CBD}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3751,7 +3685,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91FEF244-F306-4228-9F09-CA06F1ABB4CE}" type="CELLRANGE">
+                    <a:fld id="{862C1A3C-069F-4140-80CD-9886D79D9C20}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3785,7 +3719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CB00CEF-E41E-409F-B823-088DFC616586}" type="CELLRANGE">
+                    <a:fld id="{0B09E649-7F25-4AD2-BE80-15AC2E53EFA9}" type="CELLRANGE">
                       <a:rPr lang="vi-VN"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4913,155 +4847,155 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4DD68537-6844-4597-BD58-32DA7D627D44}" name="Table2" displayName="Table2" ref="A2:E6" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4DD68537-6844-4597-BD58-32DA7D627D44}" name="Table2" displayName="Table2" ref="A2:E6" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
   <autoFilter ref="A2:E6" xr:uid="{4DD68537-6844-4597-BD58-32DA7D627D44}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{343FC8A6-2B1C-40AE-BB7A-750B79CA897F}" name="Vai trò" dataDxfId="135"/>
-    <tableColumn id="2" xr3:uid="{EBEABE46-0951-4FF3-87E0-645D4C88C605}" name="Số lượng" dataDxfId="134"/>
-    <tableColumn id="3" xr3:uid="{B1DD621B-E11C-4645-BD54-CAA3DC478F02}" name="Nhiệm vụ chính" dataDxfId="133"/>
-    <tableColumn id="4" xr3:uid="{BC90AD7C-64F4-4D0C-9D39-882ECC9E5A1B}" name="Effort ước tính (%)" dataDxfId="132"/>
-    <tableColumn id="5" xr3:uid="{0701F91D-75E5-43D0-9BDE-449A7C4DE2AD}" name="Ghi chú" dataDxfId="131"/>
+    <tableColumn id="1" xr3:uid="{343FC8A6-2B1C-40AE-BB7A-750B79CA897F}" name="Vai trò" dataDxfId="126"/>
+    <tableColumn id="2" xr3:uid="{EBEABE46-0951-4FF3-87E0-645D4C88C605}" name="Số lượng" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{B1DD621B-E11C-4645-BD54-CAA3DC478F02}" name="Nhiệm vụ chính" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{BC90AD7C-64F4-4D0C-9D39-882ECC9E5A1B}" name="Effort ước tính (%)" dataDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{0701F91D-75E5-43D0-9BDE-449A7C4DE2AD}" name="Ghi chú" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{376AB492-E5A1-4986-812E-963A0468CDFE}" name="Table10" displayName="Table10" ref="A2:G9" totalsRowShown="0" headerRowDxfId="67" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{376AB492-E5A1-4986-812E-963A0468CDFE}" name="Table10" displayName="Table10" ref="A2:G9" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A2:G9" xr:uid="{376AB492-E5A1-4986-812E-963A0468CDFE}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1CABA2D0-D178-422E-AF96-CBD0E5253E88}" name="Tên công việc" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{F920DD48-FEFB-4CE4-878E-8ADDF7B93750}" name="Thời gian bắt đầu" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{417D1802-A3A4-4164-8855-A9F3CFA8530F}" name="Thời gian kết thúc" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{BA10356F-9CC9-4419-A983-B4CC7D971760}" name="Estimated Hours" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{52A99C2A-FFCF-48E6-974C-2D723EDF20A4}" name="Actual Hours" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{BA4505B4-F71B-478B-83B1-CF494FB475CD}" name="Trạng thái" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{9F83F309-FB25-4F07-A1B8-DB20D8FAB974}" name="Ghi chú" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{1CABA2D0-D178-422E-AF96-CBD0E5253E88}" name="Tên công việc" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{F920DD48-FEFB-4CE4-878E-8ADDF7B93750}" name="Thời gian bắt đầu" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{417D1802-A3A4-4164-8855-A9F3CFA8530F}" name="Thời gian kết thúc" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{BA10356F-9CC9-4419-A983-B4CC7D971760}" name="Estimated Hours" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{52A99C2A-FFCF-48E6-974C-2D723EDF20A4}" name="Actual Hours" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{BA4505B4-F71B-478B-83B1-CF494FB475CD}" name="Trạng thái" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{9F83F309-FB25-4F07-A1B8-DB20D8FAB974}" name="Ghi chú" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1BA1574A-B730-421D-8F31-1006D59B1DE7}" name="Table3" displayName="Table3" ref="G1:H6" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1BA1574A-B730-421D-8F31-1006D59B1DE7}" name="Table3" displayName="Table3" ref="G1:H6" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
   <autoFilter ref="G1:H6" xr:uid="{1BA1574A-B730-421D-8F31-1006D59B1DE7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9E82A181-17FD-43C4-969B-9FCD8C417EF6}" name="Chỉ tiêu" dataDxfId="128"/>
-    <tableColumn id="2" xr3:uid="{3CFD3F67-101F-4437-AE42-4D156D5C20FE}" name="Giá trị" dataDxfId="127"/>
+    <tableColumn id="1" xr3:uid="{9E82A181-17FD-43C4-969B-9FCD8C417EF6}" name="Chỉ tiêu" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{3CFD3F67-101F-4437-AE42-4D156D5C20FE}" name="Giá trị" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{77D8A2AE-6F7E-4419-A81C-213952C00D6A}" name="Table11" displayName="Table11" ref="B4:J26" totalsRowShown="0" headerRowDxfId="53" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{77D8A2AE-6F7E-4419-A81C-213952C00D6A}" name="Table11" displayName="Table11" ref="B4:J26" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
   <autoFilter ref="B4:J26" xr:uid="{77D8A2AE-6F7E-4419-A81C-213952C00D6A}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B9D23FBD-D4B4-4CA7-9116-7093B014876F}" name="Sprint (thời gian)" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{738EC39A-6162-466E-9889-6DAC404B2DB8}" name="Mục tiêu Sprint (Goal)" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{684C4C12-1192-444C-9A5B-D00D87F617D0}" name="Tên công việc (Task)" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{6A44603A-A7C1-4BAD-BE98-4A5ADCE46997}" name="Ngày bắt đầu" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{B342BB33-A39E-4CA4-B658-086F139F108D}" name="Ngày kết thúc" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{516059B4-AC25-4CDD-990F-07E329AE2651}" name="Estimated Hours" dataDxfId="58"/>
-    <tableColumn id="7" xr3:uid="{CE65B975-5B99-441D-9B6B-6A48974812F1}" name="Actual Hours" dataDxfId="57"/>
-    <tableColumn id="8" xr3:uid="{6B3A2A26-282E-4BDC-9AB3-92F841DC624C}" name="Trạng thái" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{C72C1436-0048-4B6F-B576-F73184224616}" name="Ghi chú" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{B9D23FBD-D4B4-4CA7-9116-7093B014876F}" name="Sprint (thời gian)" dataDxfId="115"/>
+    <tableColumn id="2" xr3:uid="{738EC39A-6162-466E-9889-6DAC404B2DB8}" name="Mục tiêu Sprint (Goal)" dataDxfId="114"/>
+    <tableColumn id="3" xr3:uid="{684C4C12-1192-444C-9A5B-D00D87F617D0}" name="Tên công việc (Task)" dataDxfId="113"/>
+    <tableColumn id="4" xr3:uid="{6A44603A-A7C1-4BAD-BE98-4A5ADCE46997}" name="Ngày bắt đầu" dataDxfId="112"/>
+    <tableColumn id="5" xr3:uid="{B342BB33-A39E-4CA4-B658-086F139F108D}" name="Ngày kết thúc" dataDxfId="111"/>
+    <tableColumn id="6" xr3:uid="{516059B4-AC25-4CDD-990F-07E329AE2651}" name="Estimated Hours" dataDxfId="110"/>
+    <tableColumn id="7" xr3:uid="{CE65B975-5B99-441D-9B6B-6A48974812F1}" name="Actual Hours" dataDxfId="109"/>
+    <tableColumn id="8" xr3:uid="{6B3A2A26-282E-4BDC-9AB3-92F841DC624C}" name="Trạng thái" dataDxfId="108"/>
+    <tableColumn id="9" xr3:uid="{C72C1436-0048-4B6F-B576-F73184224616}" name="Ghi chú" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0E9520A4-C803-4CB4-9770-B9393CB9D604}" name="Table7" displayName="Table7" ref="A2:G12" totalsRowShown="0" headerRowDxfId="64" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0E9520A4-C803-4CB4-9770-B9393CB9D604}" name="Table7" displayName="Table7" ref="A2:G12" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
   <autoFilter ref="A2:G12" xr:uid="{0E9520A4-C803-4CB4-9770-B9393CB9D604}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{839D6337-490D-4A8C-9F87-7C3332A88DD0}" name="Tên công việc" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{DC88A4E7-A37E-4DB1-B9C8-506CC523EABF}" name="Thời gian bắt đầu" dataDxfId="100"/>
-    <tableColumn id="3" xr3:uid="{06C53551-1596-4842-8943-073018D6BFF7}" name="Thời gian kết thúc" dataDxfId="99"/>
-    <tableColumn id="4" xr3:uid="{368712BB-0F7F-4EB3-9E09-0F4A9130A70E}" name="Estimated Hours" dataDxfId="98"/>
-    <tableColumn id="5" xr3:uid="{CE416111-21AF-4120-A999-F0F9C9FE8774}" name="Actual Hours" dataDxfId="97"/>
-    <tableColumn id="6" xr3:uid="{7C055D4E-A5E0-4CE6-953D-50C38F4175EC}" name="Trạng thái" dataDxfId="96"/>
-    <tableColumn id="7" xr3:uid="{855497A5-3373-4561-A028-D21468374BBC}" name="Ghi chú" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{839D6337-490D-4A8C-9F87-7C3332A88DD0}" name="Tên công việc" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{DC88A4E7-A37E-4DB1-B9C8-506CC523EABF}" name="Thời gian bắt đầu" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{06C53551-1596-4842-8943-073018D6BFF7}" name="Thời gian kết thúc" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{368712BB-0F7F-4EB3-9E09-0F4A9130A70E}" name="Estimated Hours" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{CE416111-21AF-4120-A999-F0F9C9FE8774}" name="Actual Hours" dataDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{7C055D4E-A5E0-4CE6-953D-50C38F4175EC}" name="Trạng thái" dataDxfId="99"/>
+    <tableColumn id="7" xr3:uid="{855497A5-3373-4561-A028-D21468374BBC}" name="Ghi chú" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6CEB4D39-7F5B-4364-9DD1-6200C10755AE}" name="Table6" displayName="Table6" ref="A2:G23" totalsRowShown="0" headerRowDxfId="65" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6CEB4D39-7F5B-4364-9DD1-6200C10755AE}" name="Table6" displayName="Table6" ref="A2:G23" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
   <autoFilter ref="A2:G23" xr:uid="{6CEB4D39-7F5B-4364-9DD1-6200C10755AE}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AC36644B-D872-4D32-93C2-BA79E9FA8373}" name="Tên công việc" dataDxfId="109"/>
-    <tableColumn id="2" xr3:uid="{6FE80BBE-062A-47A2-A5FB-F53FCDC8666C}" name="Thời gian bắt đầu" dataDxfId="108"/>
-    <tableColumn id="3" xr3:uid="{9B78912B-0004-4BA9-901E-E6507107B1E8}" name="Thời gian kết thúc" dataDxfId="107"/>
-    <tableColumn id="4" xr3:uid="{40157E7D-5D11-4CEF-A5BF-8BF4BD7E1F16}" name="Estimated Hours" dataDxfId="106"/>
-    <tableColumn id="5" xr3:uid="{A2790FBA-F501-446A-BAEC-AF6165C0A1FC}" name="Actual Hours" dataDxfId="105"/>
-    <tableColumn id="6" xr3:uid="{2D897EBE-C3F2-46E1-8B3D-C33D754064C4}" name="Trạng thái" dataDxfId="104"/>
-    <tableColumn id="7" xr3:uid="{16B6D43E-821C-4D00-BC8E-87BD48607EF3}" name="Ghi chú" dataDxfId="103"/>
+    <tableColumn id="1" xr3:uid="{AC36644B-D872-4D32-93C2-BA79E9FA8373}" name="Tên công việc" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{6FE80BBE-062A-47A2-A5FB-F53FCDC8666C}" name="Thời gian bắt đầu" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{9B78912B-0004-4BA9-901E-E6507107B1E8}" name="Thời gian kết thúc" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{40157E7D-5D11-4CEF-A5BF-8BF4BD7E1F16}" name="Estimated Hours" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{A2790FBA-F501-446A-BAEC-AF6165C0A1FC}" name="Actual Hours" dataDxfId="91"/>
+    <tableColumn id="6" xr3:uid="{2D897EBE-C3F2-46E1-8B3D-C33D754064C4}" name="Trạng thái" dataDxfId="90"/>
+    <tableColumn id="7" xr3:uid="{16B6D43E-821C-4D00-BC8E-87BD48607EF3}" name="Ghi chú" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6823FC75-3643-4690-8E43-C325AAE6123D}" name="Table5" displayName="Table5" ref="A2:G20" totalsRowShown="0" headerRowDxfId="66" dataDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6823FC75-3643-4690-8E43-C325AAE6123D}" name="Table5" displayName="Table5" ref="A2:G20" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87">
   <autoFilter ref="A2:G20" xr:uid="{6823FC75-3643-4690-8E43-C325AAE6123D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B6BEACDD-B393-4CED-962D-843B47CA48A4}" name="Tên công việc" dataDxfId="117"/>
-    <tableColumn id="2" xr3:uid="{3E84315E-AE71-46D0-A3BE-DAF56BF91DB1}" name="Thời gian bắt đầu" dataDxfId="116"/>
-    <tableColumn id="3" xr3:uid="{DF584D09-A819-4D71-8E78-68E924210D7E}" name="Thời gian kết thúc" dataDxfId="115"/>
-    <tableColumn id="4" xr3:uid="{09DED17E-139F-4A1E-8EA1-0A28EF66CFC9}" name="Estimated Hours" dataDxfId="114"/>
-    <tableColumn id="5" xr3:uid="{CD710DD1-1A2C-4612-9AD3-029A62B7584C}" name="Actual Hours" dataDxfId="113"/>
-    <tableColumn id="6" xr3:uid="{84EFDB02-FE21-41D6-BE34-C0F3629D8C8B}" name="Trạng thái" dataDxfId="112"/>
-    <tableColumn id="7" xr3:uid="{E9358D0E-A768-4DD4-A31E-8FCB4F36CE91}" name="Ghi chú" dataDxfId="111"/>
+    <tableColumn id="1" xr3:uid="{B6BEACDD-B393-4CED-962D-843B47CA48A4}" name="Tên công việc" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{3E84315E-AE71-46D0-A3BE-DAF56BF91DB1}" name="Thời gian bắt đầu" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{DF584D09-A819-4D71-8E78-68E924210D7E}" name="Thời gian kết thúc" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{09DED17E-139F-4A1E-8EA1-0A28EF66CFC9}" name="Estimated Hours" dataDxfId="83"/>
+    <tableColumn id="5" xr3:uid="{CD710DD1-1A2C-4612-9AD3-029A62B7584C}" name="Actual Hours" dataDxfId="82"/>
+    <tableColumn id="6" xr3:uid="{84EFDB02-FE21-41D6-BE34-C0F3629D8C8B}" name="Trạng thái" dataDxfId="81"/>
+    <tableColumn id="7" xr3:uid="{E9358D0E-A768-4DD4-A31E-8FCB4F36CE91}" name="Ghi chú" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D9DD809D-27C8-4348-ABA6-5746C6FF5D3D}" name="Table4" displayName="Table4" ref="A2:G15" totalsRowShown="0" headerRowDxfId="118" dataDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D9DD809D-27C8-4348-ABA6-5746C6FF5D3D}" name="Table4" displayName="Table4" ref="A2:G15" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
   <autoFilter ref="A2:G15" xr:uid="{D9DD809D-27C8-4348-ABA6-5746C6FF5D3D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D272ECD7-1D3E-45B4-A154-FC92FBD973B2}" name="Tên công việc" dataDxfId="126"/>
-    <tableColumn id="2" xr3:uid="{10883574-1B35-434F-9181-4DA6F7F0DD3B}" name="Thời gian bắt đầu" dataDxfId="125"/>
-    <tableColumn id="3" xr3:uid="{88852953-6FCE-4855-9231-73263C5C8597}" name="Thời gian kết thúc" dataDxfId="124"/>
-    <tableColumn id="4" xr3:uid="{54A480C7-9539-4864-972C-1AFB21A34AB9}" name="Estimated Hours" dataDxfId="123"/>
-    <tableColumn id="5" xr3:uid="{EB9D5FF8-84E9-4C94-8FD8-FE0A73150613}" name="Actual Hours" dataDxfId="122"/>
-    <tableColumn id="6" xr3:uid="{D00B9926-D151-441B-8B04-A892AAFE86B5}" name="Trạng thái" dataDxfId="121"/>
-    <tableColumn id="7" xr3:uid="{6A42BA1E-6D2B-4BC3-A12A-A36D4FCF117A}" name="Ghi chú" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{D272ECD7-1D3E-45B4-A154-FC92FBD973B2}" name="Tên công việc" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{10883574-1B35-434F-9181-4DA6F7F0DD3B}" name="Thời gian bắt đầu" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{88852953-6FCE-4855-9231-73263C5C8597}" name="Thời gian kết thúc" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{54A480C7-9539-4864-972C-1AFB21A34AB9}" name="Estimated Hours" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{EB9D5FF8-84E9-4C94-8FD8-FE0A73150613}" name="Actual Hours" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{D00B9926-D151-441B-8B04-A892AAFE86B5}" name="Trạng thái" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{6A42BA1E-6D2B-4BC3-A12A-A36D4FCF117A}" name="Ghi chú" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B3DDFBCC-95B5-4BA7-883E-5EDC1ECBEBF7}" name="Table8" displayName="Table8" ref="B2:H15" totalsRowShown="0" headerRowDxfId="85" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B3DDFBCC-95B5-4BA7-883E-5EDC1ECBEBF7}" name="Table8" displayName="Table8" ref="B2:H15" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <autoFilter ref="B2:H15" xr:uid="{B3DDFBCC-95B5-4BA7-883E-5EDC1ECBEBF7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A923EA15-4BA5-4424-A26D-AFA81CC7BCBE}" name="Tên công việc" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{C98D7C19-8C51-48F3-99FC-BDC8823F2FAC}" name="Thời gian bắt đầu" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{80AD9034-CF9E-4921-91A2-779A970AC2DA}" name="Thời gian kết thúc" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{EA6AE809-C919-4C60-8DC7-F495F34AAAF4}" name="Estimated Hours" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{D1B51102-A1E3-44ED-85A5-CE05930B10FC}" name="Actual Hours" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{3847D37F-FD79-43DD-9BEA-42FE70F6968C}" name="Trạng thái" dataDxfId="88"/>
-    <tableColumn id="7" xr3:uid="{9050A2AF-30A6-418C-97AD-8B6114626AC5}" name="Ghi chú" dataDxfId="87"/>
+    <tableColumn id="1" xr3:uid="{A923EA15-4BA5-4424-A26D-AFA81CC7BCBE}" name="Tên công việc" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{C98D7C19-8C51-48F3-99FC-BDC8823F2FAC}" name="Thời gian bắt đầu" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{80AD9034-CF9E-4921-91A2-779A970AC2DA}" name="Thời gian kết thúc" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{EA6AE809-C919-4C60-8DC7-F495F34AAAF4}" name="Estimated Hours" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{D1B51102-A1E3-44ED-85A5-CE05930B10FC}" name="Actual Hours" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{3847D37F-FD79-43DD-9BEA-42FE70F6968C}" name="Trạng thái" dataDxfId="63"/>
+    <tableColumn id="7" xr3:uid="{9050A2AF-30A6-418C-97AD-8B6114626AC5}" name="Ghi chú" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{70D98EDA-1AD2-4140-B6D2-45B30FF79C96}" name="Table9" displayName="Table9" ref="A2:G16" totalsRowShown="0" headerRowDxfId="76" dataDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{70D98EDA-1AD2-4140-B6D2-45B30FF79C96}" name="Table9" displayName="Table9" ref="A2:G16" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A2:G16" xr:uid="{70D98EDA-1AD2-4140-B6D2-45B30FF79C96}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{51DC68B7-2003-4C28-BDE4-F062320E8CE0}" name="Tên công việc" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{4E90CD56-1771-4E56-9620-CA66C9A58EF1}" name="Thời gian bắt đầu" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{AAA83DAB-F0BF-49F4-9FD1-30BD442ECE91}" name="Thời gian kết thúc" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{71635B43-8B7B-452E-B1A0-704A4BF37611}" name="Estimated Hours" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{210CDB9D-D26D-4565-AC8F-219180585E61}" name="Actual Hours" dataDxfId="80"/>
-    <tableColumn id="6" xr3:uid="{6356BDCD-A5EF-48AD-A59B-69F9587812B3}" name="Trạng thái" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{9CF3D96D-4CA9-4BE9-AA13-C9AFF4704945}" name="Ghi chú" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{51DC68B7-2003-4C28-BDE4-F062320E8CE0}" name="Tên công việc" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{4E90CD56-1771-4E56-9620-CA66C9A58EF1}" name="Thời gian bắt đầu" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{AAA83DAB-F0BF-49F4-9FD1-30BD442ECE91}" name="Thời gian kết thúc" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{71635B43-8B7B-452E-B1A0-704A4BF37611}" name="Estimated Hours" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{210CDB9D-D26D-4565-AC8F-219180585E61}" name="Actual Hours" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{6356BDCD-A5EF-48AD-A59B-69F9587812B3}" name="Trạng thái" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{9CF3D96D-4CA9-4BE9-AA13-C9AFF4704945}" name="Ghi chú" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5391,15 +5325,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -5751,19 +5685,19 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="14" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="9" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="8" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="7" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="6" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
+    <cfRule type="containsText" dxfId="5" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
       <formula>NOT(ISERROR(SEARCH("Overdue",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5796,15 +5730,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>258</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -5995,19 +5929,19 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="9" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="4" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="2" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="1" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
+    <cfRule type="containsText" dxfId="0" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
       <formula>NOT(ISERROR(SEARCH("Overdue",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6040,13 +5974,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>320</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
       <c r="G1" s="1" t="s">
         <v>321</v>
       </c>
@@ -6078,7 +6012,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>308</v>
       </c>
       <c r="B3" s="2">
@@ -6087,7 +6021,7 @@
       <c r="C3" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <v>0.4</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -6101,7 +6035,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>311</v>
       </c>
       <c r="B4" s="2">
@@ -6110,7 +6044,7 @@
       <c r="C4" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>0.25</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -6124,7 +6058,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>314</v>
       </c>
       <c r="B5" s="2">
@@ -6133,7 +6067,7 @@
       <c r="C5" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <v>0.2</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -6147,7 +6081,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>317</v>
       </c>
       <c r="B6" s="2">
@@ -6156,7 +6090,7 @@
       <c r="C6" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>0.15</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -6197,14 +6131,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="17.375" style="15" customWidth="1"/>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.25" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.375" style="16" customWidth="1"/>
+    <col min="9" max="9" width="21.375" style="15" customWidth="1"/>
     <col min="10" max="10" width="13.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
@@ -6216,64 +6150,64 @@
     <col min="19" max="19" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
@@ -6282,10 +6216,10 @@
       <c r="C2" t="s">
         <v>282</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>45901</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>45905</v>
       </c>
       <c r="F2">
@@ -6297,7 +6231,7 @@
       <c r="H2" t="s">
         <v>337</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>283</v>
       </c>
       <c r="J2">
@@ -6329,7 +6263,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
@@ -6338,10 +6272,10 @@
       <c r="C3" t="s">
         <v>285</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>45915</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>45918</v>
       </c>
       <c r="F3">
@@ -6353,7 +6287,7 @@
       <c r="H3" t="s">
         <v>332</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>286</v>
       </c>
       <c r="J3">
@@ -6385,7 +6319,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
@@ -6394,10 +6328,10 @@
       <c r="C4" t="s">
         <v>288</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>45929</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>45933</v>
       </c>
       <c r="F4">
@@ -6409,7 +6343,7 @@
       <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="15" t="s">
         <v>289</v>
       </c>
       <c r="J4">
@@ -6441,7 +6375,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
@@ -6450,10 +6384,10 @@
       <c r="C5" t="s">
         <v>291</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>45943</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>45946</v>
       </c>
       <c r="F5">
@@ -6465,7 +6399,7 @@
       <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>292</v>
       </c>
       <c r="J5">
@@ -6497,7 +6431,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -6506,10 +6440,10 @@
       <c r="C6" t="s">
         <v>294</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>45963</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>45968</v>
       </c>
       <c r="F6">
@@ -6521,7 +6455,7 @@
       <c r="H6" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="15" t="s">
         <v>295</v>
       </c>
       <c r="J6">
@@ -6553,7 +6487,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
@@ -6562,10 +6496,10 @@
       <c r="C7" t="s">
         <v>297</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>45973</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>45973</v>
       </c>
       <c r="F7">
@@ -6577,7 +6511,7 @@
       <c r="H7" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="15" t="s">
         <v>298</v>
       </c>
       <c r="J7">
@@ -6609,7 +6543,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
@@ -6618,10 +6552,10 @@
       <c r="C8" t="s">
         <v>299</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>45976</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>45980</v>
       </c>
       <c r="F8">
@@ -6633,7 +6567,7 @@
       <c r="H8" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>300</v>
       </c>
       <c r="J8">
@@ -6665,7 +6599,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
@@ -6674,10 +6608,10 @@
       <c r="C9" t="s">
         <v>302</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>45985</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>45987</v>
       </c>
       <c r="F9">
@@ -6689,7 +6623,7 @@
       <c r="H9" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="15" t="s">
         <v>303</v>
       </c>
       <c r="J9">
@@ -6721,38 +6655,38 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
+      <c r="A13" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:S1" xr:uid="{2B190B79-7B0B-45F8-BC63-F4A3316C9EF7}"/>
   <conditionalFormatting sqref="H2:H9">
-    <cfRule type="cellIs" dxfId="52" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="4" priority="5" stopIfTrue="1" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="39" priority="5" stopIfTrue="1" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" stopIfTrue="1" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="38" priority="6" stopIfTrue="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="7" stopIfTrue="1" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="37" priority="7" stopIfTrue="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="8" stopIfTrue="1" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="36" priority="8" stopIfTrue="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="9" stopIfTrue="1" operator="containsText" text="Overdue">
+    <cfRule type="containsText" dxfId="35" priority="9" stopIfTrue="1" operator="containsText" text="Overdue">
       <formula>NOT(ISERROR(SEARCH("Overdue",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6789,42 +6723,42 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="5">
@@ -6842,14 +6776,14 @@
       <c r="I5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="44.25" x14ac:dyDescent="0.2">
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="5">
@@ -6867,14 +6801,14 @@
       <c r="I6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="5">
@@ -6892,14 +6826,14 @@
       <c r="I7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="5">
@@ -6917,18 +6851,18 @@
       <c r="I8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="5">
@@ -6946,14 +6880,14 @@
       <c r="I9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="5">
@@ -6971,14 +6905,14 @@
       <c r="I10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="29.25" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="5">
@@ -6996,18 +6930,18 @@
       <c r="I11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>34</v>
       </c>
       <c r="E12" s="5">
@@ -7025,14 +6959,14 @@
       <c r="I12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="29.25" x14ac:dyDescent="0.2">
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13" t="s">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="5">
@@ -7050,14 +6984,14 @@
       <c r="I13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="5">
@@ -7075,18 +7009,18 @@
       <c r="I14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="44.25" x14ac:dyDescent="0.2">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>41</v>
       </c>
       <c r="E15" s="5">
@@ -7104,14 +7038,14 @@
       <c r="I15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="44.25" x14ac:dyDescent="0.2">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="5">
@@ -7129,14 +7063,14 @@
       <c r="I16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="29.25" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="5">
@@ -7154,18 +7088,18 @@
       <c r="I17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="44.25" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="5">
@@ -7183,14 +7117,14 @@
       <c r="I18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="43.5" x14ac:dyDescent="0.2">
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12" t="s">
         <v>50</v>
       </c>
       <c r="E19" s="5">
@@ -7208,14 +7142,14 @@
       <c r="I19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13" t="s">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="5">
@@ -7233,18 +7167,18 @@
       <c r="I20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="12" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="5">
@@ -7262,14 +7196,14 @@
       <c r="I21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J21" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="29.25" x14ac:dyDescent="0.2">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12" t="s">
         <v>57</v>
       </c>
       <c r="E22" s="5">
@@ -7287,14 +7221,14 @@
       <c r="I22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="29.25" x14ac:dyDescent="0.2">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12" t="s">
         <v>59</v>
       </c>
       <c r="E23" s="5">
@@ -7312,18 +7246,18 @@
       <c r="I23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E24" s="5">
@@ -7341,14 +7275,14 @@
       <c r="I24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="29.25" x14ac:dyDescent="0.2">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="s">
         <v>64</v>
       </c>
       <c r="E25" s="5">
@@ -7366,14 +7300,14 @@
       <c r="I25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="J25" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13" t="s">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E26" s="5">
@@ -7391,7 +7325,7 @@
       <c r="I26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="12" t="s">
         <v>67</v>
       </c>
     </row>
@@ -7428,15 +7362,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -7696,19 +7630,19 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="39" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="34" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="33" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="32" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="31" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
+    <cfRule type="containsText" dxfId="30" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
       <formula>NOT(ISERROR(SEARCH("Overdue",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7730,14 +7664,14 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="23.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.875" customWidth="1"/>
+    <col min="2" max="2" width="16.75" style="9" customWidth="1"/>
     <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.125" bestFit="1" customWidth="1"/>
@@ -7757,9 +7691,9 @@
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>175</v>
       </c>
@@ -7786,19 +7720,19 @@
       <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="24">
         <v>45915</v>
       </c>
-      <c r="C3" s="7">
-        <v>45915</v>
-      </c>
-      <c r="D3" s="8">
+      <c r="C3" s="24">
+        <v>45916</v>
+      </c>
+      <c r="D3" s="7">
         <v>4</v>
       </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>334</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -7809,19 +7743,19 @@
       <c r="A4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="24">
         <v>45916</v>
       </c>
-      <c r="C4" s="7">
-        <v>45916</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="C4" s="24">
+        <v>45917</v>
+      </c>
+      <c r="D4" s="7">
         <v>4</v>
       </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -7832,19 +7766,19 @@
       <c r="A5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="7">
-        <v>45916</v>
-      </c>
-      <c r="C5" s="7">
-        <v>45916</v>
-      </c>
-      <c r="D5" s="8">
+      <c r="B5" s="24">
+        <v>45917</v>
+      </c>
+      <c r="C5" s="24">
+        <v>45918</v>
+      </c>
+      <c r="D5" s="7">
         <v>4</v>
       </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -7855,20 +7789,20 @@
       <c r="A6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="7">
-        <v>45917</v>
-      </c>
-      <c r="C6" s="7">
-        <v>45917</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="B6" s="24">
+        <v>45918</v>
+      </c>
+      <c r="C6" s="24">
+        <v>45919</v>
+      </c>
+      <c r="D6" s="7">
         <v>4</v>
       </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>9</v>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>92</v>
@@ -7878,20 +7812,20 @@
       <c r="A7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="7">
-        <v>45917</v>
-      </c>
-      <c r="C7" s="7">
-        <v>45917</v>
-      </c>
-      <c r="D7" s="8">
+      <c r="B7" s="24">
+        <v>45919</v>
+      </c>
+      <c r="C7" s="24">
+        <v>45920</v>
+      </c>
+      <c r="D7" s="7">
         <v>4</v>
       </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>9</v>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>93</v>
@@ -7899,251 +7833,251 @@
     </row>
     <row r="8" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="7">
-        <v>45918</v>
-      </c>
-      <c r="C8" s="7">
-        <v>45918</v>
-      </c>
-      <c r="D8" s="8">
+        <v>78</v>
+      </c>
+      <c r="B8" s="24">
+        <v>45920</v>
+      </c>
+      <c r="C8" s="24">
+        <v>45921</v>
+      </c>
+      <c r="D8" s="7">
         <v>4</v>
       </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="7">
-        <v>45918</v>
-      </c>
-      <c r="C9" s="7">
-        <v>45918</v>
-      </c>
-      <c r="D9" s="8">
+        <v>73</v>
+      </c>
+      <c r="B9" s="24">
+        <v>45921</v>
+      </c>
+      <c r="C9" s="24">
+        <v>45922</v>
+      </c>
+      <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="7">
-        <v>45919</v>
-      </c>
-      <c r="C10" s="7">
-        <v>45919</v>
-      </c>
-      <c r="D10" s="8">
+        <v>74</v>
+      </c>
+      <c r="B10" s="24">
+        <v>45922</v>
+      </c>
+      <c r="C10" s="24">
+        <v>45923</v>
+      </c>
+      <c r="D10" s="7">
         <v>4</v>
       </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>9</v>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="7">
-        <v>45919</v>
-      </c>
-      <c r="C11" s="7">
-        <v>45919</v>
-      </c>
-      <c r="D11" s="8">
-        <v>4</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="24">
+        <v>45923</v>
+      </c>
+      <c r="C11" s="24">
+        <v>45924</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="7">
-        <v>45920</v>
-      </c>
-      <c r="C12" s="7">
-        <v>45920</v>
-      </c>
-      <c r="D12" s="8">
+        <v>75</v>
+      </c>
+      <c r="B12" s="24">
+        <v>45924</v>
+      </c>
+      <c r="C12" s="24">
+        <v>45925</v>
+      </c>
+      <c r="D12" s="7">
         <v>4</v>
       </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>9</v>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="7">
-        <v>45920</v>
-      </c>
-      <c r="C13" s="7">
-        <v>45920</v>
-      </c>
-      <c r="D13" s="8">
+        <v>76</v>
+      </c>
+      <c r="B13" s="24">
+        <v>45925</v>
+      </c>
+      <c r="C13" s="24">
+        <v>45926</v>
+      </c>
+      <c r="D13" s="7">
         <v>4</v>
       </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>9</v>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>332</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="7">
-        <v>45921</v>
-      </c>
-      <c r="C14" s="7">
-        <v>45921</v>
-      </c>
-      <c r="D14" s="8">
-        <v>2</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
-      <c r="F14" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="24">
+        <v>45926</v>
+      </c>
+      <c r="C14" s="24">
+        <v>45927</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="7">
-        <v>45921</v>
-      </c>
-      <c r="C15" s="7">
-        <v>45921</v>
-      </c>
-      <c r="D15" s="8">
+        <v>82</v>
+      </c>
+      <c r="B15" s="24">
+        <v>45927</v>
+      </c>
+      <c r="C15" s="24">
+        <v>45928</v>
+      </c>
+      <c r="D15" s="7">
         <v>4</v>
       </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="7">
-        <v>45922</v>
-      </c>
-      <c r="C16" s="7">
-        <v>45922</v>
-      </c>
-      <c r="D16" s="8">
+        <v>80</v>
+      </c>
+      <c r="B16" s="24">
+        <v>45928</v>
+      </c>
+      <c r="C16" s="24">
+        <v>45929</v>
+      </c>
+      <c r="D16" s="7">
         <v>4</v>
       </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="7">
-        <v>45922</v>
-      </c>
-      <c r="C17" s="7">
-        <v>45922</v>
-      </c>
-      <c r="D17" s="8">
+        <v>81</v>
+      </c>
+      <c r="B17" s="24">
+        <v>45929</v>
+      </c>
+      <c r="C17" s="24">
+        <v>45930</v>
+      </c>
+      <c r="D17" s="7">
         <v>4</v>
       </c>
-      <c r="E17" s="8">
-        <v>0</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="7">
-        <v>45923</v>
-      </c>
-      <c r="C18" s="7">
-        <v>45923</v>
-      </c>
-      <c r="D18" s="8">
+      <c r="B18" s="24">
+        <v>45930</v>
+      </c>
+      <c r="C18" s="24">
+        <v>45931</v>
+      </c>
+      <c r="D18" s="7">
         <v>5</v>
       </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -8154,19 +8088,19 @@
       <c r="A19" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="7">
-        <v>45923</v>
-      </c>
-      <c r="C19" s="7">
-        <v>45923</v>
-      </c>
-      <c r="D19" s="8">
+      <c r="B19" s="24">
+        <v>45931</v>
+      </c>
+      <c r="C19" s="24">
+        <v>45932</v>
+      </c>
+      <c r="D19" s="7">
         <v>5</v>
       </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="6" t="s">
@@ -8177,19 +8111,19 @@
       <c r="A20" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="7">
-        <v>45924</v>
-      </c>
-      <c r="C20" s="7">
-        <v>45924</v>
-      </c>
-      <c r="D20" s="8">
+      <c r="B20" s="24">
+        <v>45932</v>
+      </c>
+      <c r="C20" s="24">
+        <v>45933</v>
+      </c>
+      <c r="D20" s="7">
         <v>4</v>
       </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="8" t="s">
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="6" t="s">
@@ -8200,19 +8134,19 @@
       <c r="A21" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="7">
-        <v>45924</v>
-      </c>
-      <c r="C21" s="7">
-        <v>45924</v>
-      </c>
-      <c r="D21" s="8">
+      <c r="B21" s="24">
+        <v>45933</v>
+      </c>
+      <c r="C21" s="24">
+        <v>45934</v>
+      </c>
+      <c r="D21" s="7">
         <v>4</v>
       </c>
-      <c r="E21" s="8">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G21" s="6" t="s">
@@ -8223,19 +8157,19 @@
       <c r="A22" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="7">
-        <v>45925</v>
-      </c>
-      <c r="C22" s="7">
-        <v>45925</v>
-      </c>
-      <c r="D22" s="8">
+      <c r="B22" s="24">
+        <v>45934</v>
+      </c>
+      <c r="C22" s="24">
+        <v>45935</v>
+      </c>
+      <c r="D22" s="7">
         <v>4</v>
       </c>
-      <c r="E22" s="8">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="6" t="s">
@@ -8246,20 +8180,20 @@
       <c r="A23" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="7">
-        <v>45925</v>
-      </c>
-      <c r="C23" s="7">
-        <v>45925</v>
-      </c>
-      <c r="D23" s="8">
+      <c r="B23" s="24">
+        <v>45935</v>
+      </c>
+      <c r="C23" s="24">
+        <v>45936</v>
+      </c>
+      <c r="D23" s="7">
         <v>4</v>
       </c>
-      <c r="E23" s="8">
-        <v>0</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>9</v>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>109</v>
@@ -8270,19 +8204,19 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="34" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="29" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="28" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="27" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="26" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
+    <cfRule type="containsText" dxfId="25" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
       <formula>NOT(ISERROR(SEARCH("Overdue",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8321,15 +8255,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -8782,19 +8716,19 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="29" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="24" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="23" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="22" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="21" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
+    <cfRule type="containsText" dxfId="20" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
       <formula>NOT(ISERROR(SEARCH("Overdue",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8831,15 +8765,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -9168,19 +9102,19 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="24" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="19" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="18" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="17" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="16" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
+    <cfRule type="containsText" dxfId="15" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
       <formula>NOT(ISERROR(SEARCH("Overdue",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9218,15 +9152,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -9555,19 +9489,19 @@
     <mergeCell ref="B1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="19" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="14" priority="1" stopIfTrue="1" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="13" priority="2" stopIfTrue="1" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="12" priority="3" stopIfTrue="1" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="11" priority="4" stopIfTrue="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
+    <cfRule type="containsText" dxfId="10" priority="5" stopIfTrue="1" operator="containsText" text="Overdue">
       <formula>NOT(ISERROR(SEARCH("Overdue",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>